<commit_message>
Mind Place v1.05 (rename package) DB_VERSION = 8;
</commit_message>
<xml_diff>
--- a/MindPlace.xlsx
+++ b/MindPlace.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Задачи после релиза</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>//Анимации на LearnFragments и Activities</t>
+  </si>
+  <si>
+    <t>Добавить больше теоретических материалов (Как создавать ассоциации)</t>
   </si>
 </sst>
 </file>
@@ -535,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.25"/>
@@ -558,7 +561,7 @@
       </c>
       <c r="C1" s="2">
         <f>COUNTA(B$2:B$1048576)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -695,6 +698,14 @@
       </c>
       <c r="B18" s="4" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>